<commit_message>
McNo1, McNo2 확인 및 추가
</commit_message>
<xml_diff>
--- a/JTC_Forth/SETUP/LOS053P23_LAON_IO JTC 수동.xlsx
+++ b/JTC_Forth/SETUP/LOS053P23_LAON_IO JTC 수동.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@PROJECT\이전프로젝트\JTC (2)\쉐카이나_JTC\SETUP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@PROJECT_P\CVI2020\JTC_Forth\SETUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A778B5E1-3D39-4535-8E1C-7BF93DA2D541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD496543-BA7F-449D-B5E4-089993E8DC82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="1020">
   <si>
     <t>PLC -&gt; PC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3482,6 +3482,22 @@
   </si>
   <si>
     <t>PROBE 외경 초기/동작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하단 제품 감지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">상단 제품 감지 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NG 제품 감지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANUAL에 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4007,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M220" sqref="M220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -11915,7 +11931,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A209" t="str">
         <f t="shared" si="20"/>
         <v xml:space="preserve">M12E </v>
@@ -11948,7 +11964,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A210" t="str">
         <f t="shared" si="20"/>
         <v xml:space="preserve">M12F </v>
@@ -11981,7 +11997,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A211" t="str">
         <f t="shared" si="20"/>
         <v>M130 I/F LAMP 1</v>
@@ -12020,7 +12036,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A212" t="str">
         <f t="shared" si="20"/>
         <v>M131 I/F LAMP 2</v>
@@ -12059,7 +12075,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A213" t="str">
         <f t="shared" si="20"/>
         <v>M132 I/F LAMP 3</v>
@@ -12098,7 +12114,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A214" t="str">
         <f t="shared" si="20"/>
         <v>M133 I/F LAMP 4</v>
@@ -12137,7 +12153,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A215" t="str">
         <f t="shared" si="20"/>
         <v>M134 I/F LAMP 5</v>
@@ -12176,7 +12192,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A216" t="str">
         <f t="shared" si="20"/>
         <v>M135 I/F LAMP 6</v>
@@ -12215,7 +12231,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A217" t="str">
         <f t="shared" ref="A217:A280" si="24">_xlfn.CONCAT(C217,D217," ",F217)</f>
         <v>M136 I/F LAMP 7</v>
@@ -12254,7 +12270,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A218" t="str">
         <f t="shared" si="24"/>
         <v>M137 I/F LAMP 8</v>
@@ -12293,14 +12309,14 @@
         <v>535</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A219" t="str">
         <f t="shared" si="24"/>
         <v>M138 WORK DETECT LAMP 1</v>
       </c>
       <c r="B219" t="str">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">M338 </v>
+        <v>M338 하단 제품 감지</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>3</v>
@@ -12331,15 +12347,21 @@
         <f t="shared" si="23"/>
         <v>536</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L219" t="s">
+        <v>1016</v>
+      </c>
+      <c r="M219" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A220" t="str">
         <f t="shared" si="24"/>
         <v>M139 WORK DETECT LAMP 2</v>
       </c>
       <c r="B220" t="str">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">M339 </v>
+        <v xml:space="preserve">M339 상단 제품 감지 </v>
       </c>
       <c r="C220" s="1" t="s">
         <v>3</v>
@@ -12370,15 +12392,18 @@
         <f t="shared" si="23"/>
         <v>537</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L220" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A221" t="str">
         <f t="shared" si="24"/>
         <v>M13A WORK DETECT LAMP 3</v>
       </c>
       <c r="B221" t="str">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">M33A </v>
+        <v>M33A NG 제품 감지</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>3</v>
@@ -12409,8 +12434,11 @@
         <f t="shared" si="23"/>
         <v>538</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L221" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A222" t="str">
         <f t="shared" si="24"/>
         <v>M13B WORK DETECT LAMP 4</v>
@@ -12449,7 +12477,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A223" t="str">
         <f t="shared" si="24"/>
         <v>M13C WORK DETECT LAMP 5</v>
@@ -12488,7 +12516,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A224" t="str">
         <f t="shared" si="24"/>
         <v>M13D WORK DETECT LAMP 6</v>

</xml_diff>